<commit_message>
Figuring out entity placement from Scenario tag, Scenery done-ish
</commit_message>
<xml_diff>
--- a/Research/ScenarioResearch.xlsx
+++ b/Research/ScenarioResearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE72534F-3A91-4941-8C4A-F2473DC05482}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC45B878-D9A6-4636-835F-3BA520F6A98F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Cao Location</t>
   </si>
@@ -57,18 +57,12 @@
     <t>mostly empty, last 4 bytes is two shorts, [6,2]</t>
   </si>
   <si>
-    <t>some shorts, some floats, no obvious significance</t>
-  </si>
-  <si>
     <t>Scen tag references, padded with zeroes</t>
   </si>
   <si>
     <t>Weap tag references, padded with zeroes</t>
   </si>
   <si>
-    <t>some short enums, then 5ish floats, padding</t>
-  </si>
-  <si>
     <t>confidence</t>
   </si>
   <si>
@@ -78,18 +72,12 @@
     <t>Mach tag references, padded with zeroes</t>
   </si>
   <si>
-    <t>some short enums, then some floats, padding</t>
-  </si>
-  <si>
     <t>Ssce tag references, padded with zeroes</t>
   </si>
   <si>
     <t>Ligh tag reference, padded with zeroes</t>
   </si>
   <si>
-    <t>four floats, padded with zeroes</t>
-  </si>
-  <si>
     <t>byte sized enums/indicies, zeroes, and six floats</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
     <t>11,14,18,12</t>
   </si>
   <si>
-    <t>floats, padded with zeroes</t>
-  </si>
-  <si>
     <t>Itmc references, flags, zeroes, xyz, orientation, and tag id</t>
   </si>
   <si>
@@ -169,6 +154,39 @@
   </si>
   <si>
     <t>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</t>
+  </si>
+  <si>
+    <t>Things I need to find</t>
+  </si>
+  <si>
+    <t>Scenery spawns</t>
+  </si>
+  <si>
+    <t>Player spawns</t>
+  </si>
+  <si>
+    <t>Itmc spawns</t>
+  </si>
+  <si>
+    <t>Mach spawns</t>
+  </si>
+  <si>
+    <t>Itemc/weap placement</t>
+  </si>
+  <si>
+    <t>Ssce placement?</t>
+  </si>
+  <si>
+    <t>Light placement?</t>
+  </si>
+  <si>
+    <t>game mode markers? KotH, Flag spawns, etc</t>
+  </si>
+  <si>
+    <t>player spawn, xyz with rotation - almost certainly</t>
+  </si>
+  <si>
+    <t>definitely sword placement on zanzibar - but not on lockout, no shotgun on lockout either</t>
   </si>
 </sst>
 </file>
@@ -565,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1D70A5-77EB-4101-A684-C29A663B6757}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,11 +597,12 @@
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="102.85546875" customWidth="1"/>
     <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -601,12 +620,15 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -624,8 +646,19 @@
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"[FixedLength(" &amp; E2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
+        <v>[FixedLength(8)]public class Obj8 {}</v>
+      </c>
+      <c r="N2" t="str">
+        <f>"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(8)] public Obj8[] Obj8s { get; set; }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>72</v>
       </c>
@@ -642,8 +675,19 @@
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J34" si="1">"[FixedLength(" &amp; E3 &amp; ")]public class Obj" &amp; B3 &amp; " {}"</f>
+        <v>[FixedLength(36)]public class Obj72 {}</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N34" si="2">"[InternalReferenceValue(" &amp; B3 &amp; ")] public Obj" &amp; B3 &amp; "[] Obj" &amp; B3 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(72)] public Obj72[] Obj72s { get; set; }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>80</v>
       </c>
@@ -658,12 +702,23 @@
         <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(92)]public class Obj80 {}</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(80)] public Obj80[] Obj80s { get; set; }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>88</v>
@@ -679,12 +734,23 @@
         <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj88 {}</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(88)] public Obj88[] Obj88s { get; set; }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>152</v>
@@ -700,10 +766,18 @@
         <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj152 {}</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(152)] public Obj152[] Obj152s { get; set; }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>168</v>
       </c>
@@ -718,12 +792,20 @@
         <v>72</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(72)]public class Obj168 {}</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(168)] public Obj168[] Obj168s { get; set; }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
       </c>
       <c r="B8">
         <v>176</v>
@@ -739,10 +821,18 @@
         <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj176 {}</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(176)] public Obj176[] Obj176s { get; set; }</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>216</v>
       </c>
@@ -757,12 +847,20 @@
         <v>80</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(80)]public class Obj216 {}</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(216)] public Obj216[] Obj216s { get; set; }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>224</v>
@@ -778,10 +876,18 @@
         <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj224 {}</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(224)] public Obj224[] Obj224s { get; set; }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>232</v>
       </c>
@@ -796,12 +902,20 @@
         <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(108)]public class Obj232 {}</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(232)] public Obj232[] Obj232s { get; set; }</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>240</v>
@@ -817,10 +931,18 @@
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj240 {}</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(240)] public Obj240[] Obj240s { get; set; }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>256</v>
       </c>
@@ -835,10 +957,18 @@
         <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(52)]public class Obj256 {}</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(256)] public Obj256[] Obj256s { get; set; }</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>264</v>
       </c>
@@ -853,13 +983,21 @@
         <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(68)]public class Obj264 {}</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(264)] public Obj264[] Obj264s { get; set; }</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>280</v>
       </c>
@@ -874,12 +1012,20 @@
         <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(32)]public class Obj280 {}</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(280)] public Obj280[] Obj280s { get; set; }</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>288</v>
@@ -895,10 +1041,18 @@
         <v>144</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(144)]public class Obj288 {}</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(288)] public Obj288[] Obj288s { get; set; }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>296</v>
       </c>
@@ -913,15 +1067,23 @@
         <v>156</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G17">
         <v>3848273950</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(156)]public class Obj296 {}</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(296)] public Obj296[] Obj296s { get; set; }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>320</v>
@@ -937,12 +1099,20 @@
         <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(8)]public class Obj320 {}</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(320)] public Obj320[] Obj320s { get; set; }</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>432</v>
@@ -958,13 +1128,21 @@
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(1)]public class Obj432 {}</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(432)] public Obj432[] Obj432s { get; set; }</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>472</v>
       </c>
@@ -979,10 +1157,18 @@
         <v>128</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(128)]public class Obj472 {}</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(472)] public Obj472[] Obj472s { get; set; }</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>528</v>
       </c>
@@ -997,10 +1183,18 @@
         <v>68</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(68)]public class Obj528 {}</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(528)] public Obj528[] Obj528s { get; set; }</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>536</v>
       </c>
@@ -1015,10 +1209,18 @@
         <v>152</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(152)]public class Obj536 {}</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(536)] public Obj536[] Obj536s { get; set; }</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>560</v>
       </c>
@@ -1033,13 +1235,21 @@
         <v>2</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(2)]public class Obj560 {}</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(560)] public Obj560[] Obj560s { get; set; }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>568</v>
       </c>
@@ -1054,10 +1264,18 @@
         <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(20)]public class Obj568 {}</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(568)] public Obj568[] Obj568s { get; set; }</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>592</v>
       </c>
@@ -1072,13 +1290,21 @@
         <v>100</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(100)]public class Obj592 {}</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(592)] public Obj592[] Obj592s { get; set; }</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>600</v>
       </c>
@@ -1093,13 +1319,21 @@
         <v>72</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(72)]public class Obj600 {}</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(600)] public Obj600[] Obj600s { get; set; }</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>656</v>
       </c>
@@ -1114,10 +1348,18 @@
         <v>192</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(192)]public class Obj656 {}</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(656)] public Obj656[] Obj656s { get; set; }</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>792</v>
       </c>
@@ -1132,13 +1374,21 @@
         <v>816</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G28">
         <v>251668766</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(816)]public class Obj792 {}</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(792)] public Obj792[] Obj792s { get; set; }</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>808</v>
       </c>
@@ -1153,12 +1403,20 @@
         <v>76</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(76)]public class Obj808 {}</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(808)] public Obj808[] Obj808s { get; set; }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>816</v>
@@ -1174,10 +1432,18 @@
         <v>40</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj816 {}</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(816)] public Obj816[] Obj816s { get; set; }</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>840</v>
       </c>
@@ -1192,10 +1458,18 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(16)]public class Obj840 {}</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(840)] public Obj840[] Obj840s { get; set; }</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>904</v>
       </c>
@@ -1210,12 +1484,20 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(16)]public class Obj904 {}</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>920</v>
@@ -1231,12 +1513,20 @@
         <v>3196</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(3196)]public class Obj920 {}</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>984</v>
@@ -1252,10 +1542,18 @@
         <v>4</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(4)]public class Obj984 {}</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(984)] public Obj984[] Obj984s { get; set; }</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>32136</v>
       </c>

</xml_diff>

<commit_message>
First pass on placing instanced geometry in BSP
</commit_message>
<xml_diff>
--- a/Research/ScenarioResearch.xlsx
+++ b/Research/ScenarioResearch.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2226CADB-15EB-43C0-9631-8C72CE7BB17D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FA61C4-2F19-458C-B6C7-10BFCAE74553}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
+    <workbookView xWindow="29460" yWindow="795" windowWidth="26160" windowHeight="13995" activeTab="2" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="MixedRefs">Sheet1!$B$2:$F$61</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Cao Location</t>
   </si>
@@ -659,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1D70A5-77EB-4101-A684-C29A663B6757}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D43" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:M2"/>
     </sheetView>
   </sheetViews>
@@ -2158,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93F109B-BCDF-4565-9C8C-406C6C6EEB56}">
   <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,7 +2184,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="str">
-        <f>VLOOKUP(B1, MixedRefs,5, FALSE)</f>
+        <f t="shared" ref="F1:F6" si="1">VLOOKUP(B1, MixedRefs,5, FALSE)</f>
         <v>Skybox refs</v>
       </c>
       <c r="H1" t="str">
@@ -2209,15 +2211,15 @@
         <v>36</v>
       </c>
       <c r="F2" t="str">
-        <f>VLOOKUP(B2, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="1"/>
         <v>mostly empty, last 4 bytes is two shorts, [6,2]</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H45" si="1">"[FixedLength(" &amp; E2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
+        <f t="shared" ref="H2:H45" si="2">"[FixedLength(" &amp; E2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
         <v>[FixedLength(36)]public class Obj72 {}</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L45" si="2">"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
+        <f t="shared" ref="L2:L45" si="3">"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
         <v>[InternalReferenceValue(72)] public Obj72[] Obj72s { get; set; }</v>
       </c>
     </row>
@@ -2236,15 +2238,15 @@
         <v>92</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>VLOOKUP(B3, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="1"/>
         <v>scenery</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(92)]public class Obj80 {}</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(80)] public Obj80[] Obj80s { get; set; }</v>
       </c>
     </row>
@@ -2259,19 +2261,19 @@
         <v>4852</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E45" si="3">(D5-D4)/C4</f>
+        <f t="shared" ref="E4:E45" si="4">(D5-D4)/C4</f>
         <v>40</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>VLOOKUP(B4, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="1"/>
         <v>Scen tag references, padded with zeroes</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj88 {}</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(88)] public Obj88[] Obj88s { get; set; }</v>
       </c>
     </row>
@@ -2286,19 +2288,19 @@
         <v>5772</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="F5" t="str">
-        <f>VLOOKUP(B5, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="1"/>
         <v>[1,9]/[0,10] then four floats, plus some other data</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(84)]public class Obj96 {}</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(96)] public Obj96[] Obj96s { get; set; }</v>
       </c>
     </row>
@@ -2313,19 +2315,19 @@
         <v>5940</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F6" t="str">
-        <f>VLOOKUP(B6, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="1"/>
         <v>Bipd references</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj104 {}</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(104)] public Obj104[] Obj104s { get; set; }</v>
       </c>
     </row>
@@ -2340,18 +2342,18 @@
         <v>6020</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(84)]public class Obj144 {}</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(144)] public Obj144[] Obj144s { get; set; }</v>
       </c>
     </row>
@@ -2366,7 +2368,7 @@
         <v>6104</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F8" t="str">
@@ -2374,11 +2376,11 @@
         <v>Weap tag references, padded with zeroes</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj152 {}</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(152)] public Obj152[] Obj152s { get; set; }</v>
       </c>
     </row>
@@ -2393,7 +2395,7 @@
         <v>6144</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F9" t="str">
@@ -2401,11 +2403,11 @@
         <v>gate string</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj160 {}</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(160)] public Obj160[] Obj160s { get; set; }</v>
       </c>
     </row>
@@ -2420,18 +2422,18 @@
         <v>6184</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(72)]public class Obj168 {}</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(168)] public Obj168[] Obj168s { get; set; }</v>
       </c>
     </row>
@@ -2446,19 +2448,19 @@
         <v>6616</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F11" t="str">
-        <f>VLOOKUP(B11, MixedRefs,5, FALSE)</f>
+        <f t="shared" ref="F11:F45" si="5">VLOOKUP(B11, MixedRefs,5, FALSE)</f>
         <v>Mach tag references, padded with zeroes</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj176 {}</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(176)] public Obj176[] Obj176s { get; set; }</v>
       </c>
     </row>
@@ -2473,19 +2475,19 @@
         <v>6776</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>VLOOKUP(B12, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>floats - ctrl placement</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(68)]public class Obj184 {}</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(184)] public Obj184[] Obj184s { get; set; }</v>
       </c>
     </row>
@@ -2500,19 +2502,19 @@
         <v>6844</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F13" t="str">
-        <f>VLOOKUP(B13, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>ctrl ref</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj192 {}</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(192)] public Obj192[] Obj192s { get; set; }</v>
       </c>
     </row>
@@ -2527,19 +2529,19 @@
         <v>6884</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>VLOOKUP(B14, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Ssce placement?</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(80)]public class Obj216 {}</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(216)] public Obj216[] Obj216s { get; set; }</v>
       </c>
     </row>
@@ -2554,19 +2556,19 @@
         <v>9044</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F15" t="str">
-        <f>VLOOKUP(B15, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Ssce tag references, padded with zeroes</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj224 {}</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(224)] public Obj224[] Obj224s { get; set; }</v>
       </c>
     </row>
@@ -2581,19 +2583,19 @@
         <v>9604</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>VLOOKUP(B16, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Light placement?</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(108)]public class Obj232 {}</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(232)] public Obj232[] Obj232s { get; set; }</v>
       </c>
     </row>
@@ -2608,19 +2610,19 @@
         <v>9820</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F17" t="str">
-        <f>VLOOKUP(B17, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Ligh tag reference, padded with zeroes</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj240 {}</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(240)] public Obj240[] Obj240s { get; set; }</v>
       </c>
     </row>
@@ -2635,19 +2637,19 @@
         <v>9860</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>VLOOKUP(B18, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>player spawn, xyz with rotation - almost certainly</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(52)]public class Obj256 {}</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(256)] public Obj256[] Obj256s { get; set; }</v>
       </c>
     </row>
@@ -2662,19 +2664,19 @@
         <v>12928</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="F19" t="str">
-        <f>VLOOKUP(B19, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>byte sized enums/indicies, zeroes, and six floats</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(68)]public class Obj264 {}</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(264)] public Obj264[] Obj264s { get; set; }</v>
       </c>
     </row>
@@ -2689,19 +2691,19 @@
         <v>12996</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>VLOOKUP(B20, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>game mode markers? KotH, Flag spawns, etc</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(32)]public class Obj280 {}</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(280)] public Obj280[] Obj280s { get; set; }</v>
       </c>
     </row>
@@ -2716,19 +2718,19 @@
         <v>15300</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>VLOOKUP(B21, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Itmc references, flags, zeroes, xyz, orientation, and tag id</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(144)]public class Obj288 {}</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(288)] public Obj288[] Obj288s { get; set; }</v>
       </c>
     </row>
@@ -2743,19 +2745,19 @@
         <v>26100</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
       <c r="F22" t="str">
-        <f>VLOOKUP(B22, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Itmc refs, all null tag except first - default equip?</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(156)]public class Obj296 {}</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(296)] public Obj296[] Obj296s { get; set; }</v>
       </c>
     </row>
@@ -2770,19 +2772,19 @@
         <v>26256</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>VLOOKUP(B23, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>decal placements</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(16)]public class Obj312 {}</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(312)] public Obj312[] Obj312s { get; set; }</v>
       </c>
     </row>
@@ -2797,19 +2799,19 @@
         <v>26896</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F24" t="str">
-        <f>VLOOKUP(B24, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Deca references, tight</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(8)]public class Obj320 {}</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(320)] public Obj320[] Obj320s { get; set; }</v>
       </c>
     </row>
@@ -2824,19 +2826,19 @@
         <v>27080</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.000956937799043</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>VLOOKUP(B25, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Text</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(1.00095693779904)]public class Obj432 {}</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(432)] public Obj432[] Obj432s { get; set; }</v>
       </c>
     </row>
@@ -2851,19 +2853,19 @@
         <v>29172</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>VLOOKUP(B26, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>text with refs</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj440 {}</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(440)] public Obj440[] Obj440s { get; set; }</v>
       </c>
     </row>
@@ -2878,19 +2880,19 @@
         <v>30132</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>VLOOKUP(B27, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>same as above</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj448 {}</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(448)] public Obj448[] Obj448s { get; set; }</v>
       </c>
     </row>
@@ -2905,19 +2907,19 @@
         <v>30172</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>VLOOKUP(B28, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>All zeroes</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(128)]public class Obj472 {}</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(472)] public Obj472[] Obj472s { get; set; }</v>
       </c>
     </row>
@@ -2932,19 +2934,19 @@
         <v>30300</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="F29" t="str">
-        <f>VLOOKUP(B29, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>strings with floats</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(56)]public class Obj480 {}</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
       </c>
     </row>
@@ -2959,19 +2961,19 @@
         <v>30636</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="F30" t="str">
-        <f>VLOOKUP(B30, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>strings, floats</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(64)]public class Obj488 {}</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(488)] public Obj488[] Obj488s { get; set; }</v>
       </c>
     </row>
@@ -2986,19 +2988,19 @@
         <v>33772</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>VLOOKUP(B31, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Sbsp and lightmap tag references, maybe some flags</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(68)]public class Obj528 {}</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(528)] public Obj528[] Obj528s { get; set; }</v>
       </c>
     </row>
@@ -3013,19 +3015,19 @@
         <v>33840</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>VLOOKUP(B32, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Internal ref to a series of tag refs -&gt; *cen, *piq, refs, etc</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(168)]public class Obj536 {}</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(536)] public Obj536[] Obj536s { get; set; }</v>
       </c>
     </row>
@@ -3040,19 +3042,19 @@
         <v>34008</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>VLOOKUP(B33, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Ids as shorts?</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(4)]public class Obj560 {}</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(560)] public Obj560[] Obj560s { get; set; }</v>
       </c>
     </row>
@@ -3067,19 +3069,19 @@
         <v>34012</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="F34" t="str">
-        <f>VLOOKUP(B34, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Just 00, then 16 bytes of BA</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(20)]public class Obj568 {}</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(568)] public Obj568[] Obj568s { get; set; }</v>
       </c>
     </row>
@@ -3094,19 +3096,19 @@
         <v>58312</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="F35" t="str">
-        <f>VLOOKUP(B35, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>ascension string, then zeroes, then lsnd ref</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(100)]public class Obj592 {}</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(592)] public Obj592[] Obj592s { get; set; }</v>
       </c>
     </row>
@@ -3121,19 +3123,19 @@
         <v>58712</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="F36" t="str">
-        <f>VLOOKUP(B36, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>cliffs string, snde reference</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(72)]public class Obj600 {}</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(600)] public Obj600[] Obj600s { get; set; }</v>
       </c>
     </row>
@@ -3148,19 +3150,19 @@
         <v>58856</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1372</v>
       </c>
       <c r="F37" t="str">
-        <f>VLOOKUP(B37, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Null sbsp tagref, internal refs to subsequent values (floats)</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(1372)]public class Obj656 {}</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(656)] public Obj656[] Obj656s { get; set; }</v>
       </c>
     </row>
@@ -3175,19 +3177,19 @@
         <v>60228</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1056</v>
       </c>
       <c r="F38" t="str">
-        <f>VLOOKUP(B38, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Internal refs, 48 size blocks, then more 48 size blocks. Lots of floats</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(1056)]public class Obj792 {}</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(792)] public Obj792[] Obj792s { get; set; }</v>
       </c>
     </row>
@@ -3202,19 +3204,19 @@
         <v>61284</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>VLOOKUP(B39, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Crates and stuff</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(76)]public class Obj808 {}</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(808)] public Obj808[] Obj808s { get; set; }</v>
       </c>
     </row>
@@ -3229,19 +3231,19 @@
         <v>65920</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>VLOOKUP(B40, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>bloc ref, padded with zeroes</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj816 {}</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(816)] public Obj816[] Obj816s { get; set; }</v>
       </c>
     </row>
@@ -3256,19 +3258,19 @@
         <v>66880</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F41" t="str">
-        <f>VLOOKUP(B41, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Fog tag - ref?</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(16)]public class Obj840 {}</v>
       </c>
       <c r="L41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(840)] public Obj840[] Obj840s { get; set; }</v>
       </c>
     </row>
@@ -3283,19 +3285,19 @@
         <v>66896</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F42" t="str">
-        <f>VLOOKUP(B42, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>DECR refs</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(8)]public class Obj888 {}</v>
       </c>
       <c r="L42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(888)] public Obj888[] Obj888s { get; set; }</v>
       </c>
     </row>
@@ -3310,19 +3312,19 @@
         <v>66912</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F43" t="str">
-        <f>VLOOKUP(B43, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Empty sbsp ref</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(40)]public class Obj904 {}</v>
       </c>
       <c r="L43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
       </c>
     </row>
@@ -3337,19 +3339,19 @@
         <v>66952</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3196</v>
       </c>
       <c r="F44" t="str">
-        <f>VLOOKUP(B44, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Bitm, then utf-16 strings of the name and description of the map</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(3196)]public class Obj920 {}</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
       </c>
     </row>
@@ -3364,19 +3366,19 @@
         <v>70148</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-173.20493827160493</v>
       </c>
       <c r="F45" t="str">
-        <f>VLOOKUP(B45, MixedRefs,5, FALSE)</f>
+        <f t="shared" si="5"/>
         <v>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[FixedLength(-173.204938271605)]public class Obj984 {}</v>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>[InternalReferenceValue(984)] public Obj984[] Obj984s { get; set; }</v>
       </c>
     </row>
@@ -3384,4 +3386,1297 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50946101-636E-4CAC-9348-8C1BCC50A424}">
+  <dimension ref="B1:L40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>992</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E2" si="0">(D2-D1)/C1</f>
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f t="shared" ref="F1:F6" si="1">VLOOKUP(B1, MixedRefs,5, FALSE)</f>
+        <v>Skybox refs</v>
+      </c>
+      <c r="H1" t="str">
+        <f>"[FixedLength(" &amp; E1 &amp; ")]public class Obj" &amp; B1 &amp; " {}"</f>
+        <v>[FixedLength(8)]public class Obj8 {}</v>
+      </c>
+      <c r="L1" t="str">
+        <f>"[InternalReferenceValue(" &amp; B1 &amp; ")] public Obj" &amp; B1 &amp; "[] Obj" &amp; B1 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(8)] public Obj8[] Obj8s { get; set; }</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" si="1"/>
+        <v>scenery</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H45" si="2">"[FixedLength(" &amp; E2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
+        <v>[FixedLength(92)]public class Obj80 {}</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L45" si="3">"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(80)] public Obj80[] Obj80s { get; set; }</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3">
+        <f>(D4-D3)/C3</f>
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Scen tag references, padded with zeroes</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(40)]public class Obj88 {}</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(88)] public Obj88[] Obj88s { get; set; }</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>216</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>2492</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E45" si="4">(D5-D4)/C4</f>
+        <v>80</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Ssce placement?</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(80)]public class Obj216 {}</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(216)] public Obj216[] Obj216s { get; set; }</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>224</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4252</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>Ssce tag references, padded with zeroes</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(40)]public class Obj224 {}</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(224)] public Obj224[] Obj224s { get; set; }</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>232</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>4492</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>Light placement?</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(108)]public class Obj232 {}</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(232)] public Obj232[] Obj232s { get; set; }</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>240</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6760</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(40)]public class Obj240 {}</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(240)] public Obj240[] Obj240s { get; set; }</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>256</v>
+      </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
+      <c r="D8">
+        <v>7000</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="F8" t="str">
+        <f>VLOOKUP(B8, MixedRefs,5, FALSE)</f>
+        <v>player spawn, xyz with rotation - almost certainly</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(52)]public class Obj256 {}</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(256)] public Obj256[] Obj256s { get; set; }</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>280</v>
+      </c>
+      <c r="C9">
+        <v>78</v>
+      </c>
+      <c r="D9">
+        <v>13396</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="F9" t="str">
+        <f>VLOOKUP(B9, MixedRefs,5, FALSE)</f>
+        <v>game mode markers? KotH, Flag spawns, etc</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(32)]public class Obj280 {}</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(280)] public Obj280[] Obj280s { get; set; }</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>288</v>
+      </c>
+      <c r="C10">
+        <v>61</v>
+      </c>
+      <c r="D10">
+        <v>15892</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(144)]public class Obj288 {}</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(288)] public Obj288[] Obj288s { get; set; }</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>296</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>24676</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" ref="F11:F45" si="5">VLOOKUP(B11, MixedRefs,5, FALSE)</f>
+        <v>Itmc refs, all null tag except first - default equip?</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(156)]public class Obj296 {}</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(296)] public Obj296[] Obj296s { get; set; }</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>432</v>
+      </c>
+      <c r="C12">
+        <v>1024</v>
+      </c>
+      <c r="D12">
+        <v>24832</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Text</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(1)]public class Obj432 {}</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(432)] public Obj432[] Obj432s { get; set; }</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>472</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>25856</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="5"/>
+        <v>All zeroes</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(128)]public class Obj472 {}</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(472)] public Obj472[] Obj472s { get; set; }</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>528</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>25984</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Sbsp and lightmap tag references, maybe some flags</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(68)]public class Obj528 {}</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(528)] public Obj528[] Obj528s { get; set; }</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>568</v>
+      </c>
+      <c r="C15">
+        <v>516</v>
+      </c>
+      <c r="D15">
+        <v>26052</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="5"/>
+        <v>Just 00, then 16 bytes of BA</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(20)]public class Obj568 {}</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(568)] public Obj568[] Obj568s { get; set; }</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>592</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>36372</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ascension string, then zeroes, then lsnd ref</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(100)]public class Obj592 {}</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(592)] public Obj592[] Obj592s { get; set; }</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>600</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>36672</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="5"/>
+        <v>cliffs string, snde reference</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(72)]public class Obj600 {}</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(600)] public Obj600[] Obj600s { get; set; }</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>656</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>36960</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>1204</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Null sbsp tagref, internal refs to subsequent values (floats)</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(1204)]public class Obj656 {}</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(656)] public Obj656[] Obj656s { get; set; }</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>792</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>38164</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="5"/>
+        <v>Internal refs, 48 size blocks, then more 48 size blocks. Lots of floats</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(1056)]public class Obj792 {}</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(792)] public Obj792[] Obj792s { get; set; }</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>808</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>39220</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Crates and stuff</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(76)]public class Obj808 {}</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(808)] public Obj808[] Obj808s { get; set; }</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>816</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>39372</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>bloc ref, padded with zeroes</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(40)]public class Obj816 {}</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(816)] public Obj816[] Obj816s { get; set; }</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>888</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>39412</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="5"/>
+        <v>DECR refs</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(8)]public class Obj888 {}</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(888)] public Obj888[] Obj888s { get; set; }</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>904</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>39428</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Empty sbsp ref</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(16)]public class Obj904 {}</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>920</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>39444</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>3196</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="5"/>
+        <v>Bitm, then utf-16 strings of the name and description of the map</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(3196)]public class Obj920 {}</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>984</v>
+      </c>
+      <c r="C25">
+        <v>350</v>
+      </c>
+      <c r="D25">
+        <v>42640</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>-16.079999999999998</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(-16.08)]public class Obj984 {}</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(984)] public Obj984[] Obj984s { get; set; }</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>36968</v>
+      </c>
+      <c r="C26">
+        <v>48</v>
+      </c>
+      <c r="D26">
+        <v>37012</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(4)]public class Obj36968 {}</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(36968)] public Obj36968[] Obj36968s { get; set; }</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>36976</v>
+      </c>
+      <c r="C27">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>37204</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F27" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(4)]public class Obj36976 {}</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(36976)] public Obj36976[] Obj36976s { get; set; }</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>36988</v>
+      </c>
+      <c r="C28">
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>37396</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F28" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(12)]public class Obj36988 {}</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(36988)] public Obj36988[] Obj36988s { get; set; }</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>36996</v>
+      </c>
+      <c r="C29">
+        <v>48</v>
+      </c>
+      <c r="D29">
+        <v>37972</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(0)]public class Obj36996 {}</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(36996)] public Obj36996[] Obj36996s { get; set; }</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>37004</v>
+      </c>
+      <c r="C30">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <v>37972</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F30" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(6)]public class Obj37004 {}</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(37004)] public Obj37004[] Obj37004s { get; set; }</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>38244</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>38260</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="F31" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(48)]public class Obj38244 {}</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(38244)] public Obj38244[] Obj38244s { get; set; }</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>38252</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>38932</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>89.333333333333329</v>
+      </c>
+      <c r="F32" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(89.3333333333333)]public class Obj38252 {}</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(38252)] public Obj38252[] Obj38252s { get; set; }</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>39460</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>39468</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>-39468</v>
+      </c>
+      <c r="F33" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>[FixedLength(-39468)]public class Obj39460 {}</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="3"/>
+        <v>[InternalReferenceValue(39460)] public Obj39460[] Obj39460s { get; set; }</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F40" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A61BE83-A9AA-4FA7-880A-944707CC9C14}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>216</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>224</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>232</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>4492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>240</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>256</v>
+      </c>
+      <c r="B8">
+        <v>123</v>
+      </c>
+      <c r="C8">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>280</v>
+      </c>
+      <c r="B9">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>13396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>288</v>
+      </c>
+      <c r="B10">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>15892</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>296</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>24676</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>432</v>
+      </c>
+      <c r="B12">
+        <v>1024</v>
+      </c>
+      <c r="C12">
+        <v>24832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>472</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>25856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>528</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>25984</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>568</v>
+      </c>
+      <c r="B15">
+        <v>516</v>
+      </c>
+      <c r="C15">
+        <v>26052</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>592</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>36372</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>600</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>36672</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>656</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>36960</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>792</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>38164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>808</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>39220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>816</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>39372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>888</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>39412</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>904</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>39428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>920</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>39444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>984</v>
+      </c>
+      <c r="B25">
+        <v>350</v>
+      </c>
+      <c r="C25">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>36968</v>
+      </c>
+      <c r="B26">
+        <v>48</v>
+      </c>
+      <c r="C26">
+        <v>37012</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>36976</v>
+      </c>
+      <c r="B27">
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <v>37204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>36988</v>
+      </c>
+      <c r="B28">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <v>37396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>36996</v>
+      </c>
+      <c r="B29">
+        <v>48</v>
+      </c>
+      <c r="C29">
+        <v>37972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>37004</v>
+      </c>
+      <c r="B30">
+        <v>48</v>
+      </c>
+      <c r="C30">
+        <v>37972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>38244</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>38260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>38252</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>38932</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>39460</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>39468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Start of refactoring towards rendering extensability
</commit_message>
<xml_diff>
--- a/Research/ScenarioResearch.xlsx
+++ b/Research/ScenarioResearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2C2D9E-1E9C-47E8-AC6B-69FFE25A4C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A8830-4E30-4EF1-B37F-EEFCAE68A064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="MixedRefs">Sheet1!$B$2:$F$74</definedName>
+    <definedName name="MixedRefs">Sheet1!$B$2:$F$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Cao Location</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Not sure, fpch ref? is that a tag?</t>
+  </si>
+  <si>
+    <t>Some shorts</t>
   </si>
 </sst>
 </file>
@@ -695,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1D70A5-77EB-4101-A684-C29A663B6757}">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,18 +777,18 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E47" si="0">(D4-D3)/C3</f>
+        <f t="shared" ref="E3:E48" si="0">(D4-D3)/C3</f>
         <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I71" si="1">"[FixedLength(" &amp; E3 &amp; ")]public class Obj" &amp; B3 &amp; " {}"</f>
+        <f t="shared" ref="I3:I72" si="1">"[FixedLength(" &amp; E3 &amp; ")]public class Obj" &amp; B3 &amp; " {}"</f>
         <v>[FixedLength(36)]public class Obj72 {}</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M71" si="2">"[InternalReferenceValue(" &amp; B3 &amp; ")] public Obj" &amp; B3 &amp; "[] Obj" &amp; B3 &amp; "s { get; set; }"</f>
+        <f t="shared" ref="M3:M72" si="2">"[InternalReferenceValue(" &amp; B3 &amp; ")] public Obj" &amp; B3 &amp; "[] Obj" &amp; B3 &amp; "s { get; set; }"</f>
         <v>[InternalReferenceValue(72)] public Obj72[] Obj72s { get; set; }</v>
       </c>
     </row>
@@ -1706,74 +1709,57 @@
         <v>27532</v>
       </c>
       <c r="E44">
+        <f>(D46-D44)/C44</f>
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(16)]public class Obj840 {}</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(840)] public Obj840[] Obj840s { get; set; }</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>896</v>
+      </c>
+      <c r="F45" t="s">
+        <v>77</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(896)] public Obj896[] Obj896s { get; set; }</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>904</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>27548</v>
+      </c>
+      <c r="E46">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(16)]public class Obj840 {}</v>
-      </c>
-      <c r="M44" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(840)] public Obj840[] Obj840s { get; set; }</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>904</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>27548</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>35</v>
       </c>
-      <c r="I45" t="str">
+      <c r="I46" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(16)]public class Obj904 {}</v>
       </c>
-      <c r="M45" t="str">
+      <c r="M46" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46">
-        <v>920</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>27564</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>3196</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I46" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(3196)]public class Obj920 {}</v>
-      </c>
-      <c r="M46" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -1781,47 +1767,66 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>984</v>
+        <v>920</v>
       </c>
       <c r="C47">
-        <v>344</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>30760</v>
+        <v>27564</v>
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
+        <v>3196</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(3196)]public class Obj920 {}</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>984</v>
+      </c>
+      <c r="C48">
+        <v>344</v>
+      </c>
+      <c r="D48">
+        <v>30760</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I47" t="str">
+      <c r="I48" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(4)]public class Obj984 {}</v>
       </c>
-      <c r="M47" t="str">
+      <c r="M48" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(984)] public Obj984[] Obj984s { get; set; }</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D48">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D49">
         <v>32136</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>6</v>
       </c>
-      <c r="I48" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength()]public class Obj {}</v>
-      </c>
-      <c r="M48" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I49" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
@@ -1852,476 +1857,480 @@
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>96</v>
-      </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>5772</v>
-      </c>
-      <c r="E52">
-        <f t="shared" ref="E52:E80" si="3">(D53-D52)/C52</f>
-        <v>84</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="I52" t="str">
         <f t="shared" si="1"/>
-        <v>[FixedLength(84)]public class Obj96 {}</v>
+        <v>[FixedLength()]public class Obj {}</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(96)] public Obj96[] Obj96s { get; set; }</v>
+        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <v>5940</v>
+        <v>5772</v>
       </c>
       <c r="E53">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>46</v>
+        <f t="shared" ref="E53:E81" si="3">(D54-D53)/C53</f>
+        <v>84</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
-        <v>[FixedLength(40)]public class Obj104 {}</v>
+        <v>[FixedLength(84)]public class Obj96 {}</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(104)] public Obj104[] Obj104s { get; set; }</v>
+        <v>[InternalReferenceValue(96)] public Obj96[] Obj96s { get; set; }</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54">
+        <v>104</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>5940</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj104 {}</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(104)] public Obj104[] Obj104s { get; set; }</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55">
         <v>144</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>6020</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="3"/>
-        <v>84</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I54" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(84)]public class Obj144 {}</v>
-      </c>
-      <c r="M54" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(144)] public Obj144[] Obj144s { get; set; }</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>152</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>6104</v>
+        <v>6020</v>
       </c>
       <c r="E55">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
-        <v>[FixedLength(40)]public class Obj152 {}</v>
+        <v>[FixedLength(84)]public class Obj144 {}</v>
       </c>
       <c r="M55" t="str">
         <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(152)] public Obj152[] Obj152s { get; set; }</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(144)] public Obj144[] Obj144s { get; set; }</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
+        <v>6104</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj152 {}</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(152)] public Obj152[] Obj152s { get; set; }</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>160</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
         <v>6144</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>49</v>
       </c>
-      <c r="I56" t="str">
+      <c r="I57" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(40)]public class Obj160 {}</v>
       </c>
-      <c r="M56" t="str">
+      <c r="M57" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(160)] public Obj160[] Obj160s { get; set; }</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>168</v>
-      </c>
-      <c r="C57">
-        <v>6</v>
-      </c>
-      <c r="D57">
-        <v>6184</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="F57" t="s">
-        <v>47</v>
-      </c>
-      <c r="I57" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(72)]public class Obj168 {}</v>
-      </c>
-      <c r="M57" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(168)] public Obj168[] Obj168s { get; set; }</v>
       </c>
     </row>
     <row r="58" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58">
+        <v>168</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>6184</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="F58" t="s">
+        <v>47</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(72)]public class Obj168 {}</v>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(168)] public Obj168[] Obj168s { get; set; }</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B59">
         <v>176</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>4</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <v>6616</v>
       </c>
-      <c r="E58">
+      <c r="E59">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I58" t="str">
+      <c r="I59" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(40)]public class Obj176 {}</v>
       </c>
-      <c r="M58" t="str">
+      <c r="M59" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(176)] public Obj176[] Obj176s { get; set; }</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <v>184</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>6776</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="3"/>
-        <v>68</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I59" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(68)]public class Obj184 {}</v>
-      </c>
-      <c r="M59" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(184)] public Obj184[] Obj184s { get; set; }</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
+        <v>6776</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(68)]public class Obj184 {}</v>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(184)] public Obj184[] Obj184s { get; set; }</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>192</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
         <v>6844</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I60" t="str">
+      <c r="I61" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(40)]public class Obj192 {}</v>
       </c>
-      <c r="M60" t="str">
+      <c r="M61" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(192)] public Obj192[] Obj192s { get; set; }</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D61">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D62">
         <v>6884</v>
       </c>
-      <c r="I61" t="str">
+      <c r="I62" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M61" t="str">
+      <c r="M62" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I62" t="str">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I63" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M62" t="str">
+      <c r="M63" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64">
         <v>312</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>40</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>26256</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I63" t="str">
+      <c r="I64" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(16)]public class Obj312 {}</v>
       </c>
-      <c r="M63" t="str">
+      <c r="M64" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(312)] public Obj312[] Obj312s { get; set; }</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D64">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D65">
         <v>26896</v>
       </c>
-      <c r="I64" t="str">
+      <c r="I65" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M64" t="str">
+      <c r="M65" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I65" t="str">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I66" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M65" t="str">
+      <c r="M66" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66">
-        <v>440</v>
-      </c>
-      <c r="C66">
-        <v>24</v>
-      </c>
-      <c r="D66">
-        <v>29172</v>
-      </c>
-      <c r="E66">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F66" t="s">
-        <v>52</v>
-      </c>
-      <c r="I66" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(40)]public class Obj440 {}</v>
-      </c>
-      <c r="M66" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(440)] public Obj440[] Obj440s { get; set; }</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67">
+        <v>440</v>
+      </c>
+      <c r="C67">
+        <v>24</v>
+      </c>
+      <c r="D67">
+        <v>29172</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F67" t="s">
+        <v>52</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(40)]public class Obj440 {}</v>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(440)] public Obj440[] Obj440s { get; set; }</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68">
         <v>448</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>1</v>
       </c>
-      <c r="D67">
+      <c r="D68">
         <v>30132</v>
       </c>
-      <c r="E67">
+      <c r="E68">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" t="s">
         <v>53</v>
       </c>
-      <c r="I67" t="str">
+      <c r="I68" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(40)]public class Obj448 {}</v>
       </c>
-      <c r="M67" t="str">
+      <c r="M68" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(448)] public Obj448[] Obj448s { get; set; }</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D68">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D69">
         <v>30172</v>
       </c>
-      <c r="I68" t="str">
+      <c r="I69" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M68" t="str">
+      <c r="M69" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I69" t="str">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I70" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength()]public class Obj {}</v>
       </c>
-      <c r="M69" t="str">
+      <c r="M70" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <v>480</v>
-      </c>
-      <c r="C70">
-        <v>6</v>
-      </c>
-      <c r="D70">
-        <v>30300</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="F70" t="s">
-        <v>54</v>
-      </c>
-      <c r="G70" t="s">
-        <v>55</v>
-      </c>
-      <c r="I70" t="str">
-        <f t="shared" si="1"/>
-        <v>[FixedLength(56)]public class Obj480 {}</v>
-      </c>
-      <c r="M70" t="str">
-        <f t="shared" si="2"/>
-        <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71">
+        <v>480</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71">
+        <v>30300</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="F71" t="s">
+        <v>54</v>
+      </c>
+      <c r="G71" t="s">
+        <v>55</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(56)]public class Obj480 {}</v>
+      </c>
+      <c r="M71" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72">
         <v>488</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>49</v>
       </c>
-      <c r="D71">
+      <c r="D72">
         <v>30636</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F72" t="s">
         <v>56</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G72" t="s">
         <v>57</v>
       </c>
-      <c r="I71" t="str">
+      <c r="I72" t="str">
         <f t="shared" si="1"/>
         <v>[FixedLength(64)]public class Obj488 {}</v>
       </c>
-      <c r="M71" t="str">
+      <c r="M72" t="str">
         <f t="shared" si="2"/>
         <v>[InternalReferenceValue(488)] public Obj488[] Obj488s { get; set; }</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D72">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D73">
         <v>33772</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75">
         <v>888</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>2</v>
       </c>
-      <c r="D74">
+      <c r="D75">
         <v>66896</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D75">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D76">
         <v>66912</v>
-      </c>
-    </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E77" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
@@ -2338,6 +2347,12 @@
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E80" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
@@ -2352,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50946101-636E-4CAC-9348-8C1BCC50A424}">
   <dimension ref="B1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,9 +3846,9 @@
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="F55" t="e">
+      <c r="F55" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
+        <v>Some shorts</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="12"/>

</xml_diff>